<commit_message>
Actualización de archivos en la carpeta data - 2025-02-04 09:36:42
</commit_message>
<xml_diff>
--- a/data/Informe_Mensual_Unidades.xlsx
+++ b/data/Informe_Mensual_Unidades.xlsx
@@ -751,17 +751,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Marcos Barbosa</t>
+          <t>Christian Aguilar</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>143</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2023</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D2" s="7" t="n">
@@ -769,38 +769,38 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60:39:11</t>
+          <t>73:59:37</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>825</v>
+        <v>991.2</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>121.23</v>
+        <v>164.81</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>00:01:38</t>
+          <t>00:07:08</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>00:01:04</t>
+          <t>00:04:10</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
+          <t>00:00:23</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
           <t>00:00:00</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
       <c r="M2" s="1" t="n">
         <v>0</v>
       </c>
@@ -814,11 +814,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>87.01000000000001</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
-          <t>Dec 6 2:39PM CST</t>
+          <t>Jan 3 10:02AM CST</t>
         </is>
       </c>
       <c r="S2" s="1" t="n">
@@ -866,49 +866,49 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Adrian Caro</t>
+          <t>Gerardo Aguillón</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>142</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>FORD RANGER 2011</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>38:00:51</t>
+          <t>63:22:16</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>716.4</v>
+        <v>864.2</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>100.83</v>
+        <v>130.11</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>00:08:27</t>
+          <t>00:01:34</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>00:07:16</t>
+          <t>00:00:45</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>00:00:47</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr">
@@ -929,11 +929,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>93.01000000000001</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>Dec 6 11:15AM CST</t>
+          <t>Jan 2 5:41PM CST</t>
         </is>
       </c>
       <c r="S3" s="1" t="n">
@@ -981,54 +981,54 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Diego Cardenas</t>
+          <t>Hugo López</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>153</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>91:29:58</t>
+          <t>55:16:21</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>2040.6</v>
+        <v>859.2</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>285.43</v>
+        <v>152.03</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>00:43:05</t>
+          <t>00:07:53</t>
         </is>
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>00:23:11</t>
+          <t>00:03:04</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>00:02:47</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M4" s="1" t="n">
@@ -1044,11 +1044,11 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>90.01000000000001</v>
+        <v>73.01000000000001</v>
       </c>
       <c r="R4" s="1" t="inlineStr">
         <is>
-          <t>Dec 26 12:09PM CST</t>
+          <t>Jan 9 1:23PM CST</t>
         </is>
       </c>
       <c r="S4" s="1" t="n">
@@ -1096,54 +1096,54 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Christian Aguilar</t>
+          <t>Marcos Barbosa</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>147</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2023</t>
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>72:15:18</t>
+          <t>65:34:46</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>889</v>
+        <v>1044.9</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>160.45</v>
+        <v>142.38</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>00:06:32</t>
+          <t>00:04:35</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>00:06:13</t>
+          <t>00:02:47</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>00:01:05</t>
+          <t>00:01:21</t>
         </is>
       </c>
       <c r="L5" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="M5" s="1" t="n">
@@ -1159,11 +1159,11 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>76.01000000000001</v>
+        <v>99.01000000000001</v>
       </c>
       <c r="R5" s="1" t="inlineStr">
         <is>
-          <t>Dec 19 2:34PM CST</t>
+          <t>Jan 11 10:11AM CST</t>
         </is>
       </c>
       <c r="S5" s="1" t="n">
@@ -1211,61 +1211,61 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Daniel Iñiguez</t>
+          <t>Luis Ramirez</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>101</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>FORD F350 3MTS 2006</t>
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>94:09:30</t>
+          <t>45:19:03</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>1806.7</v>
+        <v>641.2</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>241.5</v>
+        <v>222.03</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>00:42:04</t>
+          <t>00:08:41</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>00:28:49</t>
+          <t>00:03:52</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>00:06:48</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="L6" s="1" t="inlineStr">
         <is>
-          <t>00:00:39</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="M6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O6" s="1" t="n">
         <v>0</v>
@@ -1274,11 +1274,11 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>80.01000000000001</v>
+        <v>82.01000000000001</v>
       </c>
       <c r="R6" s="1" t="inlineStr">
         <is>
-          <t>Dec 23 12:35PM CST</t>
+          <t>Jan 23 2:37PM CST</t>
         </is>
       </c>
       <c r="S6" s="1" t="n">
@@ -1326,54 +1326,54 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Hernandez</t>
+          <t>Moises Martinez</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>66:16:22</t>
+          <t>66:49:44</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>1015.9</v>
+        <v>1427</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>144.01</v>
+        <v>230.11</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>00:03:37</t>
+          <t>00:28:11</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>00:01:40</t>
+          <t>00:23:47</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:02:43</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:23</t>
         </is>
       </c>
       <c r="M7" s="1" t="n">
@@ -1389,11 +1389,11 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>61</v>
+        <v>89.01000000000001</v>
       </c>
       <c r="R7" s="1" t="inlineStr">
         <is>
-          <t>Dec 9 12:05PM CST</t>
+          <t>Jan 9 11:43AM CST</t>
         </is>
       </c>
       <c r="S7" s="1" t="n">
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="V7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" s="1" t="n">
         <v>0</v>
@@ -1441,61 +1441,61 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Luis Ramirez</t>
+          <t>Diego Cardenas</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>134</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>FORD F350 3MTS 2006</t>
+          <t>TOYOTA HILUX 2018</t>
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>39:11:46</t>
+          <t>94:23:57</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>519.5</v>
+        <v>2172.7</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>205.04</v>
+        <v>292.35</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>00:07:46</t>
+          <t>00:50:21</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>00:10:44</t>
+          <t>00:28:41</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr">
         <is>
-          <t>00:02:26</t>
+          <t>00:04:17</t>
         </is>
       </c>
       <c r="L8" s="1" t="inlineStr">
         <is>
-          <t>00:00:27</t>
+          <t>00:00:30</t>
         </is>
       </c>
       <c r="M8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O8" s="1" t="n">
         <v>0</v>
@@ -1504,11 +1504,11 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>80.01000000000001</v>
+        <v>96.01000000000001</v>
       </c>
       <c r="R8" s="1" t="inlineStr">
         <is>
-          <t>Dec 16 12:09PM CST</t>
+          <t>Jan 28 3:47PM CST</t>
         </is>
       </c>
       <c r="S8" s="1" t="n">
@@ -1556,54 +1556,54 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Hugo López</t>
+          <t>Daniel Iñiguez</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>131</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>54:00:04</t>
+          <t>91:14:56</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>842.9</v>
+        <v>1803.2</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>153.98</v>
+        <v>240.13</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>00:07:14</t>
+          <t>00:40:59</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>00:03:15</t>
+          <t>00:27:41</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:05:35</t>
         </is>
       </c>
       <c r="L9" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:33</t>
         </is>
       </c>
       <c r="M9" s="1" t="n">
@@ -1619,11 +1619,11 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>84.01000000000001</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="R9" s="1" t="inlineStr">
         <is>
-          <t>Dec 20 8:31AM CST</t>
+          <t>Jan 20 12:17PM CST</t>
         </is>
       </c>
       <c r="S9" s="1" t="n">
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="1" t="n">
         <v>0</v>
@@ -1671,74 +1671,74 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Angel Cortez</t>
+          <t>Eduardo Lopez</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>78:43:26</t>
+          <t>61:05:48</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>2191.3</v>
+        <v>1235.5</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>286.61</v>
+        <v>198.95</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
-          <t>00:36:16</t>
+          <t>00:33:48</t>
         </is>
       </c>
       <c r="J10" s="1" t="inlineStr">
         <is>
-          <t>00:28:33</t>
+          <t>00:26:55</t>
         </is>
       </c>
       <c r="K10" s="1" t="inlineStr">
         <is>
-          <t>00:06:58</t>
+          <t>00:05:08</t>
         </is>
       </c>
       <c r="L10" s="1" t="inlineStr">
         <is>
-          <t>00:02:34</t>
+          <t>00:00:40</t>
         </is>
       </c>
       <c r="M10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O10" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>83.01000000000001</v>
+        <v>97.01000000000001</v>
       </c>
       <c r="R10" s="1" t="inlineStr">
         <is>
-          <t>Dec 27 4:13PM CST</t>
+          <t>Jan 11 8:30AM CST</t>
         </is>
       </c>
       <c r="S10" s="1" t="n">
@@ -1800,47 +1800,47 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>45:55:21</t>
+          <t>68:07:42</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>879.8</v>
+        <v>1505.2</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>136.61</v>
+        <v>217.74</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>00:16:01</t>
+          <t>00:39:12</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>00:14:09</t>
+          <t>00:36:05</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr">
         <is>
-          <t>00:03:35</t>
+          <t>00:05:56</t>
         </is>
       </c>
       <c r="L11" s="1" t="inlineStr">
         <is>
-          <t>00:01:51</t>
+          <t>00:01:18</t>
         </is>
       </c>
       <c r="M11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="1" t="n">
         <v>0</v>
@@ -1849,11 +1849,11 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>91.01000000000001</v>
+        <v>93.01000000000001</v>
       </c>
       <c r="R11" s="1" t="inlineStr">
         <is>
-          <t>Dec 30 11:13AM CST</t>
+          <t>Jan 24 1:38PM CST</t>
         </is>
       </c>
       <c r="S11" s="1" t="n">
@@ -1901,17 +1901,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Kevin De La O</t>
+          <t>Angel Cortez</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>133</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>TOYOTA HILUX 2018</t>
         </is>
       </c>
       <c r="D12" s="8" t="n">
@@ -1919,56 +1919,56 @@
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>46:46:01</t>
+          <t>88:31:57</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>1073.7</v>
+        <v>2558.8</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0</v>
+        <v>337.13</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>00:37:05</t>
+          <t>00:47:29</t>
         </is>
       </c>
       <c r="J12" s="1" t="inlineStr">
         <is>
-          <t>00:24:30</t>
+          <t>00:42:19</t>
         </is>
       </c>
       <c r="K12" s="1" t="inlineStr">
         <is>
-          <t>00:06:15</t>
+          <t>00:08:30</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
         <is>
-          <t>00:01:19</t>
+          <t>00:03:17</t>
         </is>
       </c>
       <c r="M12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O12" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>90.34</v>
+        <v>96.01000000000001</v>
       </c>
       <c r="R12" s="1" t="inlineStr">
         <is>
-          <t>Dec 12 4:36PM CST</t>
+          <t>Jan 4 1:03PM CST</t>
         </is>
       </c>
       <c r="S12" s="1" t="n">
@@ -2016,54 +2016,54 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Lara</t>
+          <t>Luis Ibarra</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>148</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>WORKEN</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D13" s="8" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>56:59:38</t>
+          <t>77:57:31</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>2851.5</v>
+        <v>1823</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>673.75</v>
+        <v>241.08</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>00:03:50</t>
+          <t>00:18:02</t>
         </is>
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>00:03:03</t>
+          <t>00:13:41</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr">
         <is>
-          <t>00:01:14</t>
+          <t>00:02:02</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:28</t>
         </is>
       </c>
       <c r="M13" s="1" t="n">
@@ -2079,21 +2079,21 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>104.58</v>
+        <v>88.01000000000001</v>
       </c>
       <c r="R13" s="1" t="inlineStr">
         <is>
-          <t>Dec 18 5:03PM CST</t>
+          <t>Jan 31 12:13PM CST</t>
         </is>
       </c>
       <c r="S13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T13" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="1" t="n">
         <v>0</v>
@@ -2131,61 +2131,61 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Álvaro Zapata</t>
+          <t>Alexis Alvarado</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>145</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D14" s="8" t="n">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>96:12:00</t>
+          <t>02:00:30</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>4138</v>
+        <v>94</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>1116.66</v>
+        <v>20.56</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>00:33:03</t>
+          <t>00:00:32</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>00:37:15</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
         <is>
-          <t>00:12:41</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L14" s="1" t="inlineStr">
         <is>
-          <t>00:05:40</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O14" s="1" t="n">
         <v>0</v>
@@ -2194,11 +2194,11 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>108.01</v>
+        <v>97.01000000000001</v>
       </c>
       <c r="R14" s="1" t="inlineStr">
         <is>
-          <t>Dec 30 5:38AM CST</t>
+          <t>Jan 20 4:36PM CST</t>
         </is>
       </c>
       <c r="S14" s="1" t="n">
@@ -2246,74 +2246,74 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Luis Ibarra</t>
+          <t>Mario Ballinas</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>144</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
-        </is>
-      </c>
-      <c r="D15" s="8" t="n">
-        <v>83</v>
+          <t>TOYOTA HILUX 2021</t>
+        </is>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>87:55:42</t>
+          <t>76:38:21</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>1999.9</v>
+        <v>1993.9</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>266.96</v>
+        <v>283.53</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>00:16:05</t>
+          <t>00:52:23</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>00:10:47</t>
+          <t>00:59:57</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
         <is>
-          <t>00:00:51</t>
+          <t>00:12:58</t>
         </is>
       </c>
       <c r="L15" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:04:01</t>
         </is>
       </c>
       <c r="M15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="P15" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>88.01000000000001</v>
+        <v>132.01</v>
       </c>
       <c r="R15" s="1" t="inlineStr">
         <is>
-          <t>Dec 26 2:09PM CST</t>
+          <t>Jan 10 1:29PM CST</t>
         </is>
       </c>
       <c r="S15" s="1" t="n">
@@ -2361,29 +2361,29 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Fernando Garcia</t>
+          <t>Alberto Jimenez</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>103</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
-        </is>
-      </c>
-      <c r="D16" s="8" t="n">
-        <v>71</v>
+          <t>VAN HYUNDAI</t>
+        </is>
+      </c>
+      <c r="D16" s="9" t="n">
+        <v>67</v>
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>120:38:25</t>
+          <t>12:40:37</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>6229.7</v>
+        <v>314.4</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>0</v>
@@ -2393,42 +2393,42 @@
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>01:19:55</t>
+          <t>00:09:14</t>
         </is>
       </c>
       <c r="J16" s="1" t="inlineStr">
         <is>
-          <t>01:18:38</t>
+          <t>00:10:12</t>
         </is>
       </c>
       <c r="K16" s="1" t="inlineStr">
         <is>
-          <t>00:39:13</t>
+          <t>00:03:58</t>
         </is>
       </c>
       <c r="L16" s="1" t="inlineStr">
         <is>
-          <t>00:12:42</t>
+          <t>00:01:35</t>
         </is>
       </c>
       <c r="M16" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>101.26</v>
+        <v>113.74</v>
       </c>
       <c r="R16" s="1" t="inlineStr">
         <is>
-          <t>Dec 20 12:15PM CST</t>
+          <t>Jan 4 2:53PM CST</t>
         </is>
       </c>
       <c r="S16" s="1" t="n">
@@ -2476,87 +2476,87 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Moises Martinez</t>
+          <t>Miguel Guizar</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>150</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
-        </is>
-      </c>
-      <c r="D17" s="8" t="n">
-        <v>71</v>
+          <t>Hino 300 2024</t>
+        </is>
+      </c>
+      <c r="D17" s="9" t="n">
+        <v>63</v>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>59:21:44</t>
+          <t>147:27:18</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>1214.3</v>
+        <v>6831.4</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>205.97</v>
+        <v>890.6</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>00:22:05</t>
+          <t>01:59:20</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>00:14:35</t>
+          <t>01:40:43</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
         <is>
-          <t>00:01:55</t>
+          <t>00:30:37</t>
         </is>
       </c>
       <c r="L17" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:09:16</t>
         </is>
       </c>
       <c r="M17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>82.01000000000001</v>
+        <v>108.01</v>
       </c>
       <c r="R17" s="1" t="inlineStr">
         <is>
-          <t>Dec 27 4:25PM CST</t>
+          <t>Jan 24 4:31PM CST</t>
         </is>
       </c>
       <c r="S17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T17" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="V17" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W17" s="1" t="n">
         <v>0</v>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="AC17" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD17" s="1" t="n">
         <v>0</v>
@@ -2591,81 +2591,81 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Francisco Marquez</t>
+          <t>Kevin De La O</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+          <t>VAN HYUNDAI</t>
         </is>
       </c>
       <c r="D18" s="9" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>94:46:43</t>
+          <t>62:24:00</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>5344</v>
+        <v>1656.1</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>1510.92</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>01:24:01</t>
+          <t>00:46:05</t>
         </is>
       </c>
       <c r="J18" s="1" t="inlineStr">
         <is>
-          <t>01:14:35</t>
+          <t>00:42:59</t>
         </is>
       </c>
       <c r="K18" s="1" t="inlineStr">
         <is>
-          <t>00:55:02</t>
+          <t>00:09:06</t>
         </is>
       </c>
       <c r="L18" s="1" t="inlineStr">
         <is>
-          <t>00:06:51</t>
+          <t>00:04:03</t>
         </is>
       </c>
       <c r="M18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N18" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="O18" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="P18" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Q18" s="1" t="n">
-        <v>100.01</v>
+        <v>114.02</v>
       </c>
       <c r="R18" s="1" t="inlineStr">
         <is>
-          <t>Dec 7 11:19AM CST</t>
+          <t>Jan 3 2:57PM CST</t>
         </is>
       </c>
       <c r="S18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T18" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="1" t="n">
         <v>0</v>
@@ -2706,74 +2706,74 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Miguel Guizar</t>
+          <t>Alberto Sanchez</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>Hino 300 2024</t>
+          <t>VW DELIVERY 10.6</t>
         </is>
       </c>
       <c r="D19" s="9" t="n">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>150:45:04</t>
+          <t>113:24:30</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>6714.1</v>
+        <v>6466.3</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>844.2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>02:01:43</t>
+          <t>02:04:20</t>
         </is>
       </c>
       <c r="J19" s="1" t="inlineStr">
         <is>
-          <t>01:49:04</t>
+          <t>01:58:41</t>
         </is>
       </c>
       <c r="K19" s="1" t="inlineStr">
         <is>
-          <t>00:38:23</t>
+          <t>01:08:06</t>
         </is>
       </c>
       <c r="L19" s="1" t="inlineStr">
         <is>
-          <t>00:08:49</t>
+          <t>00:17:00</t>
         </is>
       </c>
       <c r="M19" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>111.01</v>
+        <v>102.83</v>
       </c>
       <c r="R19" s="1" t="inlineStr">
         <is>
-          <t>Dec 23 2:16PM CST</t>
+          <t>Jan 11 10:45AM CST</t>
         </is>
       </c>
       <c r="S19" s="1" t="n">
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="V19" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W19" s="1" t="n">
         <v>0</v>
@@ -2809,10 +2809,10 @@
         <v>0</v>
       </c>
       <c r="AC19" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD19" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE19" s="1" t="n">
         <v>0</v>
@@ -2821,81 +2821,81 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Lopez</t>
+          <t>Francisco Marquez</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>135</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
         </is>
       </c>
       <c r="D20" s="9" t="n">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>53:02:17</t>
+          <t>93:18:09</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>1015.5</v>
+        <v>5156.6</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>168.36</v>
+        <v>1411.43</v>
       </c>
       <c r="H20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="inlineStr">
+        <is>
+          <t>01:10:57</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>01:30:30</t>
+        </is>
+      </c>
+      <c r="K20" s="1" t="inlineStr">
+        <is>
+          <t>01:07:52</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="inlineStr">
+        <is>
+          <t>00:14:02</t>
+        </is>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="P20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="1" t="inlineStr">
-        <is>
-          <t>00:31:45</t>
-        </is>
-      </c>
-      <c r="J20" s="1" t="inlineStr">
-        <is>
-          <t>00:22:54</t>
-        </is>
-      </c>
-      <c r="K20" s="1" t="inlineStr">
-        <is>
-          <t>00:04:17</t>
-        </is>
-      </c>
-      <c r="L20" s="1" t="inlineStr">
-        <is>
-          <t>00:00:24</t>
-        </is>
-      </c>
-      <c r="M20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="Q20" s="1" t="n">
-        <v>94.01000000000001</v>
+        <v>98.01000000000001</v>
       </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
-          <t>Dec 12 12:33PM CST</t>
+          <t>Jan 7 6:52PM CST</t>
         </is>
       </c>
       <c r="S20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T20" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20" s="1" t="n">
         <v>0</v>
@@ -2936,84 +2936,84 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Gerardo Aguillón</t>
+          <t>Alejandro Lara</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>110</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>WORKEN</t>
         </is>
       </c>
       <c r="D21" s="9" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>61:23:33</t>
+          <t>85:49:03</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>831.7</v>
+        <v>4333.5</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>123.67</v>
+        <v>1045.42</v>
       </c>
       <c r="H21" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I21" s="1" t="inlineStr">
+        <is>
+          <t>00:20:19</t>
+        </is>
+      </c>
+      <c r="J21" s="1" t="inlineStr">
+        <is>
+          <t>00:21:19</t>
+        </is>
+      </c>
+      <c r="K21" s="1" t="inlineStr">
+        <is>
+          <t>00:11:37</t>
+        </is>
+      </c>
+      <c r="L21" s="1" t="inlineStr">
+        <is>
+          <t>00:03:55</t>
+        </is>
+      </c>
+      <c r="M21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="1" t="inlineStr">
-        <is>
-          <t>00:00:16</t>
-        </is>
-      </c>
-      <c r="J21" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="K21" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="L21" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M21" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="N21" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>54</v>
+        <v>100.77</v>
       </c>
       <c r="R21" s="1" t="inlineStr">
         <is>
-          <t>Dec 9 12:42PM CST</t>
+          <t>Jan 4 4:22PM CST</t>
         </is>
       </c>
       <c r="S21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T21" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U21" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V21" s="1" t="n">
         <v>0</v>
@@ -3051,54 +3051,54 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Alberto Jimenez</t>
+          <t>Adrian Caro</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>FORD RANGER 2011</t>
         </is>
       </c>
       <c r="D22" s="9" t="n">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>99:35:24</t>
+          <t>54:45:07</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>2495.3</v>
+        <v>1110.2</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>0</v>
+        <v>151.46</v>
       </c>
       <c r="H22" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>01:02:05</t>
+          <t>00:27:18</t>
         </is>
       </c>
       <c r="J22" s="1" t="inlineStr">
         <is>
-          <t>00:59:38</t>
+          <t>00:19:30</t>
         </is>
       </c>
       <c r="K22" s="1" t="inlineStr">
         <is>
-          <t>00:21:10</t>
+          <t>00:04:16</t>
         </is>
       </c>
       <c r="L22" s="1" t="inlineStr">
         <is>
-          <t>00:06:30</t>
+          <t>00:01:32</t>
         </is>
       </c>
       <c r="M22" s="1" t="n">
@@ -3108,33 +3108,33 @@
         <v>0</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1" t="n">
+        <v>130.01</v>
+      </c>
+      <c r="R22" s="1" t="inlineStr">
+        <is>
+          <t>Jan 25 9:25AM CST</t>
+        </is>
+      </c>
+      <c r="S22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="Q22" s="1" t="n">
-        <v>121.51</v>
-      </c>
-      <c r="R22" s="1" t="inlineStr">
-        <is>
-          <t>Dec 19 2:49PM CST</t>
-        </is>
-      </c>
-      <c r="S22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="U22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W22" s="1" t="n">
-        <v>0</v>
       </c>
       <c r="X22" s="1" t="n">
         <v>0</v>
@@ -3166,87 +3166,87 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Martin Quezada</t>
+          <t>Armando Muñoz</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>102</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>INTERNACIONAL</t>
+          <t>HINO 300</t>
         </is>
       </c>
       <c r="D23" s="9" t="n">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>107:24:17</t>
+          <t>133:43:52</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>5004.6</v>
+        <v>5725.1</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>1930.61</v>
+        <v>751.8099999999999</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>01:21:19</t>
+          <t>02:01:31</t>
         </is>
       </c>
       <c r="J23" s="1" t="inlineStr">
         <is>
-          <t>01:30:31</t>
+          <t>02:10:34</t>
         </is>
       </c>
       <c r="K23" s="1" t="inlineStr">
         <is>
-          <t>01:14:50</t>
+          <t>01:07:41</t>
         </is>
       </c>
       <c r="L23" s="1" t="inlineStr">
         <is>
-          <t>00:10:17</t>
+          <t>00:24:50</t>
         </is>
       </c>
       <c r="M23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="N23" s="1" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="O23" s="1" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="P23" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>103.01</v>
+        <v>93.01000000000001</v>
       </c>
       <c r="R23" s="1" t="inlineStr">
         <is>
-          <t>Dec 28 12:15PM CST</t>
+          <t>Jan 27 9:24AM CST</t>
         </is>
       </c>
       <c r="S23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T23" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U23" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V23" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W23" s="1" t="n">
         <v>0</v>
@@ -3272,7 +3272,7 @@
         <v>0</v>
       </c>
       <c r="AD23" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE23" s="1" t="n">
         <v>0</v>
@@ -3281,93 +3281,93 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Mario Ballinas</t>
+          <t>Fernando Garcia</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="D24" s="9" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>83:17:07</t>
+          <t>119:41:21</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>2603.9</v>
+        <v>5708.2</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>355.68</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>01:59:50</t>
+          <t>01:49:35</t>
         </is>
       </c>
       <c r="J24" s="1" t="inlineStr">
         <is>
-          <t>02:11:56</t>
+          <t>02:01:53</t>
         </is>
       </c>
       <c r="K24" s="1" t="inlineStr">
         <is>
-          <t>00:49:06</t>
+          <t>01:06:37</t>
         </is>
       </c>
       <c r="L24" s="1" t="inlineStr">
         <is>
-          <t>00:19:14</t>
+          <t>00:29:01</t>
         </is>
       </c>
       <c r="M24" s="1" t="n">
         <v>3</v>
       </c>
       <c r="N24" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P24" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>133.01</v>
+        <v>105.08</v>
       </c>
       <c r="R24" s="1" t="inlineStr">
         <is>
-          <t>Dec 19 1:43PM CST</t>
+          <t>Jan 7 1:15PM CST</t>
         </is>
       </c>
       <c r="S24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="U24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X24" s="1" t="n">
-        <v>0</v>
       </c>
       <c r="Y24" s="1" t="inlineStr">
         <is>
@@ -3396,88 +3396,88 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Armando Muñoz</t>
+          <t>Alejandro Suarez</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>146</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D25" s="9" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>135:56:23</t>
+          <t>83:05:50</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>6053.1</v>
+        <v>4693</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>772.8200000000001</v>
+        <v>1111.63</v>
       </c>
       <c r="H25" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I25" s="1" t="inlineStr">
         <is>
-          <t>02:15:31</t>
+          <t>01:07:36</t>
         </is>
       </c>
       <c r="J25" s="1" t="inlineStr">
         <is>
-          <t>02:40:50</t>
+          <t>01:57:27</t>
         </is>
       </c>
       <c r="K25" s="1" t="inlineStr">
         <is>
-          <t>00:52:13</t>
+          <t>00:38:17</t>
         </is>
       </c>
       <c r="L25" s="1" t="inlineStr">
         <is>
-          <t>00:33:13</t>
+          <t>00:22:40</t>
         </is>
       </c>
       <c r="M25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P25" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q25" s="1" t="n">
+        <v>105.01</v>
+      </c>
+      <c r="R25" s="1" t="inlineStr">
+        <is>
+          <t>Jan 11 7:28PM CST</t>
+        </is>
+      </c>
+      <c r="S25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="N25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="O25" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="P25" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q25" s="1" t="n">
-        <v>93.01000000000001</v>
-      </c>
-      <c r="R25" s="1" t="inlineStr">
-        <is>
-          <t>Dec 19 6:35AM CST</t>
-        </is>
-      </c>
-      <c r="S25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="W25" s="1" t="n">
         <v>0</v>
       </c>
@@ -3499,10 +3499,10 @@
         <v>0</v>
       </c>
       <c r="AC25" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD25" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE25" s="1" t="n">
         <v>0</v>
@@ -3511,74 +3511,74 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sanchez</t>
+          <t>Luis Galindo</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>118</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>VW DELIVERY 10.6</t>
+          <t>KENWORTH 2009</t>
         </is>
       </c>
       <c r="D26" s="9" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>126:39:24</t>
+          <t>78:27:56</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>7061.3</v>
+        <v>4113.4</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>0</v>
+        <v>1067.67</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
-          <t>02:39:46</t>
+          <t>01:05:02</t>
         </is>
       </c>
       <c r="J26" s="1" t="inlineStr">
         <is>
-          <t>02:21:31</t>
+          <t>02:05:45</t>
         </is>
       </c>
       <c r="K26" s="1" t="inlineStr">
         <is>
-          <t>01:29:24</t>
+          <t>00:42:24</t>
         </is>
       </c>
       <c r="L26" s="1" t="inlineStr">
         <is>
-          <t>00:37:16</t>
+          <t>00:21:54</t>
         </is>
       </c>
       <c r="M26" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="O26" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>101.75</v>
+        <v>96.01000000000001</v>
       </c>
       <c r="R26" s="1" t="inlineStr">
         <is>
-          <t>Dec 11 1:43PM CST</t>
+          <t>Jan 17 3:36PM CST</t>
         </is>
       </c>
       <c r="S26" s="1" t="n">
@@ -3591,13 +3591,13 @@
         <v>0</v>
       </c>
       <c r="V26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="X26" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y26" s="1" t="inlineStr">
         <is>
@@ -3626,54 +3626,54 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>José Morales</t>
+          <t>Eduardo Hernandez</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>152</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D27" s="9" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>65:21:06</t>
+          <t>79:04:08</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>1339.1</v>
+        <v>1500.7</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>180.22</v>
+        <v>190.96</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>00:31:26</t>
+          <t>00:14:21</t>
         </is>
       </c>
       <c r="J27" s="1" t="inlineStr">
         <is>
-          <t>00:14:19</t>
+          <t>00:11:17</t>
         </is>
       </c>
       <c r="K27" s="1" t="inlineStr">
         <is>
-          <t>00:02:56</t>
+          <t>00:08:52</t>
         </is>
       </c>
       <c r="L27" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:01:37</t>
         </is>
       </c>
       <c r="M27" s="1" t="n">
@@ -3683,17 +3683,17 @@
         <v>0</v>
       </c>
       <c r="O27" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>89.01000000000001</v>
+        <v>88.01000000000001</v>
       </c>
       <c r="R27" s="1" t="inlineStr">
         <is>
-          <t>Dec 10 5:16PM CST</t>
+          <t>Jan 20 2:07PM CST</t>
         </is>
       </c>
       <c r="S27" s="1" t="n">
@@ -3706,7 +3706,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W27" s="1" t="n">
         <v>0</v>
@@ -3732,7 +3732,7 @@
         <v>2</v>
       </c>
       <c r="AD27" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE27" s="1" t="n">
         <v>0</v>
@@ -3741,84 +3741,84 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Miguel Zamora</t>
+          <t>Martin Quezada</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>122</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>INTERNACIONAL</t>
         </is>
       </c>
       <c r="D28" s="9" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>113:46:46</t>
+          <t>92:18:30</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>4737</v>
+        <v>4365</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>0</v>
+        <v>1556.91</v>
       </c>
       <c r="H28" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I28" s="1" t="inlineStr">
+        <is>
+          <t>00:55:57</t>
+        </is>
+      </c>
+      <c r="J28" s="1" t="inlineStr">
+        <is>
+          <t>01:16:53</t>
+        </is>
+      </c>
+      <c r="K28" s="1" t="inlineStr">
+        <is>
+          <t>00:51:57</t>
+        </is>
+      </c>
+      <c r="L28" s="1" t="inlineStr">
+        <is>
+          <t>00:14:41</t>
+        </is>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="P28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>102.01</v>
+      </c>
+      <c r="R28" s="1" t="inlineStr">
+        <is>
+          <t>Jan 21 6:05AM CST</t>
+        </is>
+      </c>
+      <c r="S28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I28" s="1" t="inlineStr">
-        <is>
-          <t>01:52:43</t>
-        </is>
-      </c>
-      <c r="J28" s="1" t="inlineStr">
-        <is>
-          <t>02:19:52</t>
-        </is>
-      </c>
-      <c r="K28" s="1" t="inlineStr">
-        <is>
-          <t>00:56:29</t>
-        </is>
-      </c>
-      <c r="L28" s="1" t="inlineStr">
-        <is>
-          <t>00:35:52</t>
-        </is>
-      </c>
-      <c r="M28" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="N28" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="O28" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P28" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q28" s="1" t="n">
-        <v>105.35</v>
-      </c>
-      <c r="R28" s="1" t="inlineStr">
-        <is>
-          <t>Dec 4 3:42PM CST</t>
-        </is>
-      </c>
-      <c r="S28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="U28" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" s="1" t="n">
         <v>0</v>
@@ -3827,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="X28" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y28" s="1" t="inlineStr">
         <is>
@@ -3856,74 +3856,74 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Suarez</t>
+          <t>Miguel Zamora</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="D29" s="9" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>86:56:52</t>
+          <t>120:37:01</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>4788.1</v>
+        <v>5565.2</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>1142.97</v>
+        <v>0</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="inlineStr">
         <is>
-          <t>01:52:05</t>
+          <t>02:25:24</t>
         </is>
       </c>
       <c r="J29" s="1" t="inlineStr">
         <is>
-          <t>01:36:19</t>
+          <t>02:46:12</t>
         </is>
       </c>
       <c r="K29" s="1" t="inlineStr">
         <is>
-          <t>00:55:42</t>
+          <t>01:09:21</t>
         </is>
       </c>
       <c r="L29" s="1" t="inlineStr">
         <is>
-          <t>00:33:52</t>
+          <t>00:42:13</t>
         </is>
       </c>
       <c r="M29" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P29" s="1" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>104.01</v>
+        <v>110.08</v>
       </c>
       <c r="R29" s="1" t="inlineStr">
         <is>
-          <t>Dec 12 1:32PM CST</t>
+          <t>Jan 8 6:17PM CST</t>
         </is>
       </c>
       <c r="S29" s="1" t="n">
@@ -3936,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W29" s="1" t="n">
         <v>0</v>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="AD29" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE29" s="1" t="n">
         <v>0</v>
@@ -3971,17 +3971,17 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Luis Galindo</t>
+          <t>Jorge Tornero</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>117</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH 2009</t>
+          <t>HINO 300</t>
         </is>
       </c>
       <c r="D30" s="9" t="n">
@@ -3989,70 +3989,70 @@
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>97:32:02</t>
+          <t>69:57:40</t>
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>4689.9</v>
+        <v>2370</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>1267.6</v>
+        <v>252.09</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I30" s="1" t="inlineStr">
         <is>
-          <t>01:32:57</t>
+          <t>00:35:58</t>
         </is>
       </c>
       <c r="J30" s="1" t="inlineStr">
         <is>
-          <t>03:05:37</t>
+          <t>00:25:47</t>
         </is>
       </c>
       <c r="K30" s="1" t="inlineStr">
         <is>
-          <t>01:07:14</t>
+          <t>00:08:12</t>
         </is>
       </c>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t>00:43:19</t>
+          <t>00:03:47</t>
         </is>
       </c>
       <c r="M30" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="P30" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>97.01000000000001</v>
+        <v>120.01</v>
       </c>
       <c r="R30" s="1" t="inlineStr">
         <is>
-          <t>Dec 7 6:06AM CST</t>
+          <t>Jan 13 11:55AM CST</t>
         </is>
       </c>
       <c r="S30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="U30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V30" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="W30" s="1" t="n">
         <v>0</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="AC30" s="1" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AD30" s="1" t="n">
         <v>0</v>
@@ -4086,17 +4086,17 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Jorge Tornero</t>
+          <t>Abraham Arana</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D31" s="9" t="n">
@@ -4104,92 +4104,92 @@
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>94:44:13</t>
+          <t>74:33:08</t>
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>2620</v>
+        <v>1959.7</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>263.94</v>
+        <v>284.33</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I31" s="1" t="inlineStr">
         <is>
-          <t>00:51:53</t>
+          <t>00:58:59</t>
         </is>
       </c>
       <c r="J31" s="1" t="inlineStr">
         <is>
-          <t>00:32:38</t>
+          <t>01:08:22</t>
         </is>
       </c>
       <c r="K31" s="1" t="inlineStr">
         <is>
-          <t>00:05:07</t>
+          <t>00:21:22</t>
         </is>
       </c>
       <c r="L31" s="1" t="inlineStr">
         <is>
-          <t>00:02:51</t>
+          <t>00:12:39</t>
         </is>
       </c>
       <c r="M31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>122.01</v>
+      </c>
+      <c r="R31" s="1" t="inlineStr">
+        <is>
+          <t>Jan 10 3:35PM CST</t>
+        </is>
+      </c>
+      <c r="S31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N31" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="O31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" s="1" t="n">
+      <c r="W31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Q31" s="1" t="n">
-        <v>113.01</v>
-      </c>
-      <c r="R31" s="1" t="inlineStr">
-        <is>
-          <t>Dec 6 7:20AM CST</t>
-        </is>
-      </c>
-      <c r="S31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" s="1" t="n">
+      <c r="Y31" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="Z31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="W31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="Z31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="1" t="n">
-        <v>7</v>
       </c>
       <c r="AD31" s="1" t="n">
         <v>0</v>
@@ -4201,17 +4201,17 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Abraham Arana</t>
+          <t>Álvaro Zapata</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>124</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>KENWORTH</t>
         </is>
       </c>
       <c r="D32" s="9" t="n">
@@ -4219,75 +4219,75 @@
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>78:07:32</t>
+          <t>40:34:37</t>
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>2142.5</v>
+        <v>1738.7</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>290.54</v>
+        <v>483.96</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I32" s="1" t="inlineStr">
         <is>
-          <t>01:16:08</t>
+          <t>00:17:27</t>
         </is>
       </c>
       <c r="J32" s="1" t="inlineStr">
         <is>
-          <t>01:11:25</t>
+          <t>00:20:51</t>
         </is>
       </c>
       <c r="K32" s="1" t="inlineStr">
         <is>
-          <t>00:16:46</t>
+          <t>00:12:20</t>
         </is>
       </c>
       <c r="L32" s="1" t="inlineStr">
         <is>
-          <t>00:09:53</t>
+          <t>00:06:03</t>
         </is>
       </c>
       <c r="M32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N32" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="O32" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1" t="n">
+        <v>109.01</v>
+      </c>
+      <c r="R32" s="1" t="inlineStr">
+        <is>
+          <t>Jan 7 3:28AM CST</t>
+        </is>
+      </c>
+      <c r="S32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Q32" s="1" t="n">
-        <v>121.01</v>
-      </c>
-      <c r="R32" s="1" t="inlineStr">
-        <is>
-          <t>Dec 5 2:17PM CST</t>
-        </is>
-      </c>
-      <c r="S32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T32" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="U32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="V32" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="X32" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y32" s="1" t="inlineStr">
         <is>
@@ -4316,17 +4316,17 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Emmanuel Salcedo</t>
+          <t>José Morales</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D33" s="9" t="n">
@@ -4334,36 +4334,36 @@
       </c>
       <c r="E33" s="1" t="inlineStr">
         <is>
-          <t>77:45:06</t>
+          <t>66:12:49</t>
         </is>
       </c>
       <c r="F33" s="1" t="n">
-        <v>1302.9</v>
+        <v>1475.5</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>246.29</v>
+        <v>185.92</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I33" s="1" t="inlineStr">
         <is>
-          <t>00:21:36</t>
+          <t>00:35:20</t>
         </is>
       </c>
       <c r="J33" s="1" t="inlineStr">
         <is>
-          <t>00:19:09</t>
+          <t>00:20:04</t>
         </is>
       </c>
       <c r="K33" s="1" t="inlineStr">
         <is>
-          <t>00:05:28</t>
+          <t>00:04:31</t>
         </is>
       </c>
       <c r="L33" s="1" t="inlineStr">
         <is>
-          <t>00:01:44</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="M33" s="1" t="n">
@@ -4379,11 +4379,11 @@
         <v>0</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>100.01</v>
+        <v>104.01</v>
       </c>
       <c r="R33" s="1" t="inlineStr">
         <is>
-          <t>Dec 9 4:45PM CST</t>
+          <t>Jan 16 6:07PM CST</t>
         </is>
       </c>
       <c r="S33" s="1" t="n">
@@ -4396,13 +4396,13 @@
         <v>1</v>
       </c>
       <c r="V33" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W33" s="1" t="n">
         <v>0</v>
       </c>
       <c r="X33" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y33" s="1" t="inlineStr">
         <is>
@@ -4419,7 +4419,7 @@
         <v>0</v>
       </c>
       <c r="AC33" s="1" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="AD33" s="1" t="n">
         <v>0</v>
@@ -4449,43 +4449,43 @@
       </c>
       <c r="E34" s="1" t="inlineStr">
         <is>
-          <t>58:28:19</t>
+          <t>60:13:53</t>
         </is>
       </c>
       <c r="F34" s="1" t="n">
-        <v>1204.1</v>
+        <v>1149.9</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>186.76</v>
+        <v>183.95</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I34" s="1" t="inlineStr">
         <is>
-          <t>00:33:28</t>
+          <t>00:26:14</t>
         </is>
       </c>
       <c r="J34" s="1" t="inlineStr">
         <is>
-          <t>00:26:53</t>
+          <t>00:23:10</t>
         </is>
       </c>
       <c r="K34" s="1" t="inlineStr">
         <is>
-          <t>00:06:39</t>
+          <t>00:06:15</t>
         </is>
       </c>
       <c r="L34" s="1" t="inlineStr">
         <is>
-          <t>00:00:59</t>
+          <t>00:00:54</t>
         </is>
       </c>
       <c r="M34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" s="1" t="n">
         <v>0</v>
@@ -4494,11 +4494,11 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>101.01</v>
+        <v>102.01</v>
       </c>
       <c r="R34" s="1" t="inlineStr">
         <is>
-          <t>Dec 16 2:37PM CST</t>
+          <t>Jan 13 2:53PM CST</t>
         </is>
       </c>
       <c r="S34" s="1" t="n">
@@ -4511,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="V34" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W34" s="1" t="n">
         <v>0</v>
@@ -4534,7 +4534,7 @@
         <v>0</v>
       </c>
       <c r="AC34" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AD34" s="1" t="n">
         <v>0</v>
@@ -4546,174 +4546,132 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Alberto Compras</t>
+          <t>Emmanuel Salcedo</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>132</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>NISSAN 1993</t>
-        </is>
-      </c>
-      <c r="D35" s="10" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="E35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="F35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="G35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="H35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="I35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="J35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="K35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="L35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="M35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="N35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="O35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="P35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Q35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="R35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="S35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="T35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="U35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="V35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="W35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="X35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Y35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Z35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AA35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AB35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AC35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AD35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AE35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
+          <t>TOYOTA HILUX 2017</t>
+        </is>
+      </c>
+      <c r="D35" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>58:16:56</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>1093.7</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>199.24</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="I35" s="1" t="inlineStr">
+        <is>
+          <t>00:24:13</t>
+        </is>
+      </c>
+      <c r="J35" s="1" t="inlineStr">
+        <is>
+          <t>00:24:02</t>
+        </is>
+      </c>
+      <c r="K35" s="1" t="inlineStr">
+        <is>
+          <t>00:09:14</t>
+        </is>
+      </c>
+      <c r="L35" s="1" t="inlineStr">
+        <is>
+          <t>00:02:53</t>
+        </is>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <v>107.01</v>
+      </c>
+      <c r="R35" s="1" t="inlineStr">
+        <is>
+          <t>Jan 27 2:43PM CST</t>
+        </is>
+      </c>
+      <c r="S35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="U35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="W35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y35" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="Z35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Alexis Alvarado</t>
+          <t>Alberto Compras</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>115</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
+          <t>NISSAN 1993</t>
         </is>
       </c>
       <c r="D36" s="10" t="inlineStr">

</xml_diff>

<commit_message>
Actualización de archivos en la carpeta data - 2025-04-03 12:10:19
</commit_message>
<xml_diff>
--- a/data/Informe_Mensual_Unidades.xlsx
+++ b/data/Informe_Mensual_Unidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="323">
   <si>
     <t>Operador</t>
   </si>
@@ -150,6 +150,30 @@
     <t>Mar 7 8:35AM CST</t>
   </si>
   <si>
+    <t>Daniel Magallanes</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2017</t>
+  </si>
+  <si>
+    <t>51:36:38</t>
+  </si>
+  <si>
+    <t>00:02:17</t>
+  </si>
+  <si>
+    <t>00:02:51</t>
+  </si>
+  <si>
+    <t>00:01:24</t>
+  </si>
+  <si>
+    <t>Mar 25 5:30PM CST</t>
+  </si>
+  <si>
     <t>Marcos Barbosa</t>
   </si>
   <si>
@@ -399,9 +423,6 @@
     <t>130</t>
   </si>
   <si>
-    <t>TOYOTA HILUX 2017</t>
-  </si>
-  <si>
     <t>83:32:32</t>
   </si>
   <si>
@@ -783,9 +804,6 @@
     <t>00:05:28</t>
   </si>
   <si>
-    <t>00:02:51</t>
-  </si>
-  <si>
     <t>00:00:39</t>
   </si>
   <si>
@@ -885,6 +903,54 @@
     <t>Mar 10 1:59PM CST</t>
   </si>
   <si>
+    <t>David Serrano</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>52:16:21</t>
+  </si>
+  <si>
+    <t>00:34:59</t>
+  </si>
+  <si>
+    <t>00:45:28</t>
+  </si>
+  <si>
+    <t>00:14:42</t>
+  </si>
+  <si>
+    <t>00:05:43</t>
+  </si>
+  <si>
+    <t>Mar 3 1:14PM CST</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>52:02:18</t>
+  </si>
+  <si>
+    <t>00:32:15</t>
+  </si>
+  <si>
+    <t>00:36:51</t>
+  </si>
+  <si>
+    <t>00:09:18</t>
+  </si>
+  <si>
+    <t>00:04:17</t>
+  </si>
+  <si>
+    <t>Mar 28 10:18AM CST</t>
+  </si>
+  <si>
     <t>Fernando Ornelas</t>
   </si>
   <si>
@@ -922,19 +988,13 @@
   </si>
   <si>
     <t>117</t>
-  </si>
-  <si>
-    <t>TALLER</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -951,13 +1011,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1004,7 +1057,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1022,9 +1075,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1045,8 +1095,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="InformeTable" displayName="InformeTable" ref="A1:AE36">
-  <autoFilter ref="A1:AE36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="InformeTable" displayName="InformeTable" ref="A1:AE39">
+  <autoFilter ref="A1:AE39"/>
   <tableColumns count="31">
     <tableColumn id="1" name="Operador"/>
     <tableColumn id="2" name="Número de unidad"/>
@@ -1369,11 +1419,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE36"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A31" sqref="A31"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,10 +1762,10 @@
         <v>46</v>
       </c>
       <c r="F4" s="1">
-        <v>814.6</v>
+        <v>839.6</v>
       </c>
       <c r="G4" s="1">
-        <v>120.4</v>
+        <v>70.91</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1745,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>81.010000000000005</v>
+        <v>86.01</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>50</v>
@@ -1801,16 +1851,16 @@
         <v>53</v>
       </c>
       <c r="D5" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F5" s="1">
-        <v>110</v>
+        <v>814.6</v>
       </c>
       <c r="G5" s="1">
-        <v>32.68</v>
+        <v>120.4</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -1822,7 +1872,7 @@
         <v>56</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>36</v>
@@ -1831,7 +1881,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
@@ -1840,10 +1890,10 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1">
-        <v>82.01</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
@@ -1887,58 +1937,58 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F6" s="1">
-        <v>1436.3</v>
+        <v>110</v>
       </c>
       <c r="G6" s="1">
-        <v>347.47</v>
+        <v>32.68</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>82.01</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>69.010000000000005</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="S6" s="1">
         <v>0</v>
@@ -1982,41 +2032,41 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D7" s="2">
         <v>97</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1436.3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>347.47</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="1">
-        <v>182.3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>24.36</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="M7" s="1">
         <v>0</v>
       </c>
@@ -2030,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1">
-        <v>88.01</v>
+        <v>69.010000000000005</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>74</v>
@@ -2086,16 +2136,16 @@
         <v>77</v>
       </c>
       <c r="D8" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="1">
-        <v>2046.4</v>
+        <v>182.3</v>
       </c>
       <c r="G8" s="1">
-        <v>301.41000000000003</v>
+        <v>24.36</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -2110,7 +2160,7 @@
         <v>81</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -2125,7 +2175,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <v>94.01</v>
+        <v>88.01</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>82</v>
@@ -2187,10 +2237,10 @@
         <v>86</v>
       </c>
       <c r="F9" s="1">
-        <v>1326.5</v>
+        <v>2046.4</v>
       </c>
       <c r="G9" s="1">
-        <v>210.18</v>
+        <v>301.41000000000003</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -2205,25 +2255,25 @@
         <v>89</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>94.01</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>108.01</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -2267,25 +2317,25 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F10" s="1">
-        <v>1294</v>
+        <v>1326.5</v>
       </c>
       <c r="G10" s="1">
-        <v>185.89</v>
+        <v>210.18</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -2300,25 +2350,25 @@
         <v>97</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" s="1">
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>77.010000000000005</v>
+        <v>108.01</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -2362,55 +2412,55 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F11" s="1">
-        <v>1436.7</v>
+        <v>1294</v>
       </c>
       <c r="G11" s="1">
-        <v>201.95</v>
+        <v>185.89</v>
       </c>
       <c r="H11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="M11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
       </c>
       <c r="O11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="1">
         <v>0</v>
       </c>
       <c r="Q11" s="1">
-        <v>96.01</v>
+        <v>77.010000000000005</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>106</v>
@@ -2425,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="V11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11" s="1">
         <v>0</v>
@@ -2463,22 +2513,22 @@
         <v>108</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F12" s="1">
-        <v>2518.6</v>
+        <v>1436.7</v>
       </c>
       <c r="G12" s="1">
-        <v>339.33</v>
+        <v>201.95</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>110</v>
@@ -2493,7 +2543,7 @@
         <v>113</v>
       </c>
       <c r="M12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="1">
         <v>1</v>
@@ -2505,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <v>90.01</v>
+        <v>96.01</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>114</v>
@@ -2520,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="V12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="1">
         <v>0</v>
@@ -2558,34 +2608,34 @@
         <v>116</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="2">
+        <v>92</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="2">
-        <v>91</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1">
+        <v>2518.6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>339.33</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="1">
-        <v>1770.6</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
@@ -2600,10 +2650,10 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1">
-        <v>122.43</v>
+        <v>90.01</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S13" s="1">
         <v>0</v>
@@ -2647,58 +2697,58 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="2">
+        <v>91</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="3">
-        <v>89</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1">
+        <v>1770.6</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F14" s="1">
-        <v>1925.2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>262.69</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>122.43</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>5</v>
-      </c>
-      <c r="O14" s="1">
-        <v>1</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>95.01</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="S14" s="1">
         <v>0</v>
@@ -2742,58 +2792,58 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3">
+        <v>89</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="F15" s="1">
+        <v>1925.2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>262.69</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="3">
-        <v>87</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F15" s="1">
-        <v>2100.6999999999998</v>
-      </c>
-      <c r="G15" s="1">
-        <v>279.32</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="M15" s="1">
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="1">
         <v>95.01</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S15" s="1">
         <v>0</v>
@@ -2837,40 +2887,40 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="3">
+        <v>87</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="3">
-        <v>79</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1">
+        <v>2100.6999999999998</v>
+      </c>
+      <c r="G16" s="1">
+        <v>279.32</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="1">
-        <v>1821.1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>247.5</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="M16" s="1">
         <v>0</v>
@@ -2879,22 +2929,22 @@
         <v>2</v>
       </c>
       <c r="O16" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="1">
-        <v>79.010000000000005</v>
+        <v>95.01</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S16" s="1">
         <v>0</v>
       </c>
       <c r="T16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" s="1">
         <v>0</v>
@@ -2932,46 +2982,46 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="3">
+        <v>79</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="3">
-        <v>78</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="F17" s="1">
-        <v>2030.5</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>302</v>
+        <v>1821.1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>247.5</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="M17" s="1">
         <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O17" s="1">
         <v>0</v>
@@ -2980,7 +3030,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>104.5</v>
+        <v>79.010000000000005</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>156</v>
@@ -3033,58 +3083,58 @@
         <v>158</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="3">
+        <v>78</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D18" s="3">
-        <v>75</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1">
+        <v>2030.5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F18" s="1">
-        <v>5205.2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>703.43</v>
-      </c>
-      <c r="H18" s="1">
-        <v>2</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>104.5</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M18" s="1">
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
         <v>1</v>
-      </c>
-      <c r="N18" s="1">
-        <v>17</v>
-      </c>
-      <c r="O18" s="1">
-        <v>2</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>92.01</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="S18" s="1">
-        <v>0</v>
-      </c>
-      <c r="T18" s="1">
-        <v>0</v>
       </c>
       <c r="U18" s="1">
         <v>0</v>
@@ -3114,7 +3164,7 @@
         <v>0</v>
       </c>
       <c r="AD18" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE18" s="1">
         <v>0</v>
@@ -3122,58 +3172,58 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="D19" s="3">
         <v>75</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F19" s="1">
-        <v>391.6</v>
+        <v>5205.2</v>
       </c>
       <c r="G19" s="1">
-        <v>167.61</v>
+        <v>703.43</v>
       </c>
       <c r="H19" s="1">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L19" s="1" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="M19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O19" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="1">
-        <v>76.010000000000005</v>
+        <v>92.01</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="S19" s="1">
         <v>0</v>
@@ -3185,7 +3235,7 @@
         <v>0</v>
       </c>
       <c r="V19" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W19" s="1">
         <v>0</v>
@@ -3209,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="AD19" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE19" s="1">
         <v>0</v>
@@ -3217,59 +3267,59 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D20" s="3">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F20" s="1">
-        <v>5776.3</v>
+        <v>391.6</v>
       </c>
       <c r="G20" s="1">
-        <v>1598.42</v>
+        <v>167.61</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="K20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>76.010000000000005</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="M20" s="1">
-        <v>7</v>
-      </c>
-      <c r="N20" s="1">
-        <v>5</v>
-      </c>
-      <c r="O20" s="1">
-        <v>3</v>
-      </c>
-      <c r="P20" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>101.01</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="S20" s="1">
         <v>0</v>
       </c>
@@ -3280,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="V20" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W20" s="1">
         <v>0</v>
@@ -3312,58 +3362,58 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="D21" s="3">
+        <v>74</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="F21" s="1">
+        <v>5776.3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1598.42</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="4">
-        <v>67</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F21" s="1">
-        <v>338.2</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="M21" s="1">
+        <v>7</v>
+      </c>
+      <c r="N21" s="1">
+        <v>5</v>
+      </c>
+      <c r="O21" s="1">
+        <v>3</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>101.01</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="M21" s="1">
-        <v>1</v>
-      </c>
-      <c r="N21" s="1">
-        <v>8</v>
-      </c>
-      <c r="O21" s="1">
-        <v>2</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>100.92</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="S21" s="1">
         <v>0</v>
@@ -3407,28 +3457,28 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D22" s="4">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>191</v>
       </c>
       <c r="F22" s="1">
-        <v>873</v>
+        <v>338.2</v>
       </c>
       <c r="G22" s="1">
-        <v>147.84</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>192</v>
@@ -3440,31 +3490,31 @@
         <v>194</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+      <c r="N22" s="1">
+        <v>8</v>
+      </c>
+      <c r="O22" s="1">
+        <v>2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>100.92</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="M22" s="1">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>78.010000000000005</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="S22" s="1">
         <v>0</v>
       </c>
       <c r="T22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" s="1">
         <v>0</v>
@@ -3502,67 +3552,67 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="4">
+        <v>61</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="F23" s="1">
+        <v>873</v>
+      </c>
+      <c r="G23" s="1">
+        <v>147.84</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D23" s="4">
-        <v>59</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F23" s="1">
-        <v>5601.9</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1465.12</v>
-      </c>
-      <c r="H23" s="1">
-        <v>5</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>78.010000000000005</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="M23" s="1">
-        <v>0</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <v>0</v>
-      </c>
-      <c r="P23" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>109.01</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="S23" s="1">
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V23" s="1">
         <v>0</v>
@@ -3586,10 +3636,10 @@
         <v>0</v>
       </c>
       <c r="AC23" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD23" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE23" s="1">
         <v>0</v>
@@ -3597,70 +3647,70 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="D24" s="4">
+        <v>59</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D24" s="4">
-        <v>58</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="F24" s="1">
-        <v>6796.4</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>302</v>
+        <v>5601.9</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1465.12</v>
       </c>
       <c r="H24" s="1">
         <v>5</v>
       </c>
       <c r="I24" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>109.01</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M24" s="1">
-        <v>2</v>
-      </c>
-      <c r="N24" s="1">
-        <v>2</v>
-      </c>
-      <c r="O24" s="1">
-        <v>2</v>
-      </c>
-      <c r="P24" s="1">
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
         <v>1</v>
       </c>
-      <c r="Q24" s="1">
-        <v>103.5</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="S24" s="1">
-        <v>0</v>
-      </c>
-      <c r="T24" s="1">
-        <v>0</v>
-      </c>
-      <c r="U24" s="1">
-        <v>0</v>
-      </c>
       <c r="V24" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W24" s="1">
         <v>0</v>
@@ -3681,10 +3731,10 @@
         <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD24" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE24" s="1">
         <v>0</v>
@@ -3692,59 +3742,59 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="D25" s="4">
+        <v>58</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D25" s="4">
-        <v>55</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="F25" s="1">
-        <v>5574.8</v>
+        <v>6796.4</v>
       </c>
       <c r="G25" s="1">
-        <v>1392.28</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1">
         <v>5</v>
       </c>
       <c r="I25" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="M25" s="1">
+        <v>2</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2</v>
+      </c>
+      <c r="P25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>103.5</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="M25" s="1">
-        <v>3</v>
-      </c>
-      <c r="N25" s="1">
-        <v>38</v>
-      </c>
-      <c r="O25" s="1">
-        <v>8</v>
-      </c>
-      <c r="P25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>107.01</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="S25" s="1">
         <v>0</v>
       </c>
@@ -3752,10 +3802,10 @@
         <v>0</v>
       </c>
       <c r="U25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V25" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W25" s="1">
         <v>0</v>
@@ -3776,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="AC25" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD25" s="1">
         <v>0</v>
@@ -3787,59 +3837,59 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="D26" s="4">
+        <v>55</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D26" s="4">
-        <v>50</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1">
+        <v>5574.8</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1392.28</v>
+      </c>
+      <c r="H26" s="1">
+        <v>5</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F26" s="1">
-        <v>6287.3</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1">
+        <v>3</v>
+      </c>
+      <c r="N26" s="1">
+        <v>38</v>
+      </c>
+      <c r="O26" s="1">
+        <v>8</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>107.01</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="M26" s="1">
-        <v>2</v>
-      </c>
-      <c r="N26" s="1">
-        <v>18</v>
-      </c>
-      <c r="O26" s="1">
-        <v>3</v>
-      </c>
-      <c r="P26" s="1">
-        <v>5</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>100.72</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="S26" s="1">
         <v>0</v>
       </c>
@@ -3847,10 +3897,10 @@
         <v>0</v>
       </c>
       <c r="U26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W26" s="1">
         <v>0</v>
@@ -3882,58 +3932,58 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="4">
+        <v>50</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="4">
-        <v>33</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1">
+        <v>6287.3</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="F27" s="1">
-        <v>4488.7</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1002.55</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1">
+        <v>2</v>
+      </c>
+      <c r="N27" s="1">
+        <v>18</v>
+      </c>
+      <c r="O27" s="1">
+        <v>3</v>
+      </c>
+      <c r="P27" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>100.72</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="M27" s="1">
-        <v>4</v>
-      </c>
-      <c r="N27" s="1">
-        <v>10</v>
-      </c>
-      <c r="O27" s="1">
-        <v>12</v>
-      </c>
-      <c r="P27" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>103.01</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="S27" s="1">
         <v>0</v>
@@ -3977,58 +4027,58 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="4">
+        <v>33</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="F28" s="1">
+        <v>4488.7</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1002.55</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D28" s="4">
-        <v>27</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F28" s="1">
-        <v>4525</v>
-      </c>
-      <c r="G28" s="1">
-        <v>496.3</v>
-      </c>
-      <c r="H28" s="1">
-        <v>2</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="M28" s="1">
+        <v>4</v>
+      </c>
+      <c r="N28" s="1">
+        <v>10</v>
+      </c>
+      <c r="O28" s="1">
+        <v>12</v>
+      </c>
+      <c r="P28" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>103.01</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="M28" s="1">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1">
-        <v>1</v>
-      </c>
-      <c r="O28" s="1">
-        <v>3</v>
-      </c>
-      <c r="P28" s="1">
-        <v>8</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>123.01</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
@@ -4061,7 +4111,7 @@
         <v>0</v>
       </c>
       <c r="AC28" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD28" s="1">
         <v>0</v>
@@ -4072,59 +4122,59 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="4">
+        <v>27</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D29" s="4">
-        <v>23</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="F29" s="1">
-        <v>840.9</v>
+        <v>4525</v>
       </c>
       <c r="G29" s="1">
-        <v>153.08000000000001</v>
+        <v>496.3</v>
       </c>
       <c r="H29" s="1">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1">
+        <v>3</v>
+      </c>
+      <c r="P29" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>123.01</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M29" s="1">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>73.010000000000005</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="S29" s="1">
         <v>0</v>
       </c>
@@ -4141,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="X29" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y29" s="1" t="s">
         <v>36</v>
@@ -4156,7 +4206,7 @@
         <v>0</v>
       </c>
       <c r="AC29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD29" s="1">
         <v>0</v>
@@ -4167,59 +4217,59 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D30" s="4">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>259</v>
       </c>
       <c r="F30" s="1">
-        <v>2591.9</v>
+        <v>840.9</v>
       </c>
       <c r="G30" s="1">
-        <v>351.6</v>
+        <v>153.08000000000001</v>
       </c>
       <c r="H30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>260</v>
       </c>
       <c r="J30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>73.010000000000005</v>
+      </c>
+      <c r="R30" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="M30" s="1">
-        <v>0</v>
-      </c>
-      <c r="N30" s="1">
-        <v>12</v>
-      </c>
-      <c r="O30" s="1">
-        <v>3</v>
-      </c>
-      <c r="P30" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>121.01</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="S30" s="1">
         <v>0</v>
       </c>
@@ -4236,7 +4286,7 @@
         <v>0</v>
       </c>
       <c r="X30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y30" s="1" t="s">
         <v>36</v>
@@ -4262,59 +4312,59 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="F31" s="1">
+        <v>2591.9</v>
+      </c>
+      <c r="G31" s="1">
+        <v>351.6</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F31" s="1">
-        <v>1323.6</v>
-      </c>
-      <c r="G31" s="1">
-        <v>229.64</v>
-      </c>
-      <c r="H31" s="1">
-        <v>65</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>12</v>
+      </c>
+      <c r="O31" s="1">
+        <v>3</v>
+      </c>
+      <c r="P31" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>121.01</v>
+      </c>
+      <c r="R31" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="M31" s="1">
-        <v>0</v>
-      </c>
-      <c r="N31" s="1">
-        <v>0</v>
-      </c>
-      <c r="O31" s="1">
-        <v>1</v>
-      </c>
-      <c r="P31" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>107.01</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="S31" s="1">
         <v>0</v>
       </c>
@@ -4322,10 +4372,10 @@
         <v>0</v>
       </c>
       <c r="U31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V31" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W31" s="1">
         <v>0</v>
@@ -4346,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="AC31" s="1">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="AD31" s="1">
         <v>0</v>
@@ -4357,70 +4407,70 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="F32" s="1">
+        <v>1323.6</v>
+      </c>
+      <c r="G32" s="1">
+        <v>229.64</v>
+      </c>
+      <c r="H32" s="1">
+        <v>65</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F32" s="1">
-        <v>1321.1</v>
-      </c>
-      <c r="G32" s="1">
-        <v>231.73</v>
-      </c>
-      <c r="H32" s="1">
-        <v>5</v>
-      </c>
-      <c r="I32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0</v>
+      </c>
+      <c r="O32" s="1">
+        <v>1</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>107.01</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="M32" s="1">
-        <v>0</v>
-      </c>
-      <c r="N32" s="1">
-        <v>0</v>
-      </c>
-      <c r="O32" s="1">
-        <v>0</v>
-      </c>
-      <c r="P32" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>94.01</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="S32" s="1">
         <v>0</v>
       </c>
       <c r="T32" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W32" s="1">
         <v>0</v>
@@ -4441,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="AC32" s="1">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="AD32" s="1">
         <v>0</v>
@@ -4452,64 +4502,64 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="F33" s="1">
+        <v>1321.1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>231.73</v>
+      </c>
+      <c r="H33" s="1">
+        <v>5</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F33" s="1">
-        <v>1226.5</v>
-      </c>
-      <c r="G33" s="1">
-        <v>182.01</v>
-      </c>
-      <c r="H33" s="1">
-        <v>4</v>
-      </c>
-      <c r="I33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>94.01</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M33" s="1">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1">
-        <v>0</v>
-      </c>
-      <c r="O33" s="1">
-        <v>0</v>
-      </c>
-      <c r="P33" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>90.01</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="S33" s="1">
         <v>0</v>
       </c>
       <c r="T33" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U33" s="1">
         <v>0</v>
@@ -4536,7 +4586,7 @@
         <v>0</v>
       </c>
       <c r="AC33" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD33" s="1">
         <v>0</v>
@@ -4547,58 +4597,58 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1">
+        <v>1226.5</v>
+      </c>
+      <c r="G34" s="1">
+        <v>182.01</v>
+      </c>
+      <c r="H34" s="1">
+        <v>4</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="F34" s="1">
-        <v>921.2</v>
-      </c>
-      <c r="G34" s="1">
-        <v>144.31</v>
-      </c>
-      <c r="H34" s="1">
-        <v>2</v>
-      </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>90.01</v>
+      </c>
+      <c r="R34" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M34" s="1">
-        <v>0</v>
-      </c>
-      <c r="N34" s="1">
-        <v>0</v>
-      </c>
-      <c r="O34" s="1">
-        <v>0</v>
-      </c>
-      <c r="P34" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="1">
-        <v>95.01</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="S34" s="1">
         <v>0</v>
@@ -4631,7 +4681,7 @@
         <v>0</v>
       </c>
       <c r="AC34" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD34" s="1">
         <v>0</v>
@@ -4642,199 +4692,483 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="F35" s="1">
+        <v>1042.2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>92.92</v>
+      </c>
+      <c r="H35" s="1">
+        <v>9</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="J35" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="R35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="S35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="T35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="U35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="V35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="W35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="X35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="Y35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="Z35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AA35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AC35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AD35" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AE35" s="6" t="s">
-        <v>298</v>
+      <c r="K35" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>116.01</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
+        <v>7</v>
+      </c>
+      <c r="U35" s="1">
+        <v>2</v>
+      </c>
+      <c r="V35" s="1">
+        <v>0</v>
+      </c>
+      <c r="W35" s="1">
+        <v>0</v>
+      </c>
+      <c r="X35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="M36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="N36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="P36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="R36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="S36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="T36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="U36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="V36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="W36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="X36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="Y36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="Z36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AA36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AB36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AC36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AD36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AE36" s="6" t="s">
-        <v>298</v>
+        <v>45</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F36" s="1">
+        <v>997.2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>92.53</v>
+      </c>
+      <c r="H36" s="1">
+        <v>7</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>106.01</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>7</v>
+      </c>
+      <c r="U36" s="1">
+        <v>0</v>
+      </c>
+      <c r="V36" s="1">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0</v>
+      </c>
+      <c r="X36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F37" s="1">
+        <v>921.2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>144.31</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>95.01</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1">
+        <v>0</v>
+      </c>
+      <c r="U37" s="1">
+        <v>0</v>
+      </c>
+      <c r="V37" s="1">
+        <v>0</v>
+      </c>
+      <c r="W37" s="1">
+        <v>0</v>
+      </c>
+      <c r="X37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="R38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="S38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="U38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="V38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="W38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="X38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AB38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AC38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AD38" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AE38" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="T39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="U39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="W39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="X39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AB39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AC39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AD39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AE39" s="6" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>